<commit_message>
se realizo cambios de rutas, cambios en el diseño, y mensaje de bienvenida para el usuario
</commit_message>
<xml_diff>
--- a/app/Plantillas.json/Entrada/Libro2.xlsx
+++ b/app/Plantillas.json/Entrada/Libro2.xlsx
@@ -744,13 +744,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DEA3F6D-777D-477F-943A-36369F112295}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{396BB6A2-EF5D-4E07-96EC-BE522D97D7C1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{196B461F-36D9-4ECF-A136-73773A381713}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A641C9CA-7729-493B-968F-C68966E9EC82}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{717E3D43-6AE8-431C-B910-168C5EBFEC56}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43B3294B-84A3-4776-B3AD-9E846DCC667F}"/>
 </file>
</xml_diff>